<commit_message>
renaming industry by site
</commit_message>
<xml_diff>
--- a/dist/dummy_files/wiat_locations.xlsx
+++ b/dist/dummy_files/wiat_locations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jsalo\PhpstormProjects\wiat_front\public\dummy_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jsalo\Desktop\ICRA\WIAT_front\public\dummy_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ABD1CDF-C54D-4D0B-96BB-1D756F4EB5DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AF69FC1-9D2C-41DD-A5B6-2F415CA4841C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12220" xr2:uid="{60B8F55B-90B2-41A0-953E-FD593A0D51DC}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12220" activeTab="1" xr2:uid="{60B8F55B-90B2-41A0-953E-FD593A0D51DC}"/>
   </bookViews>
   <sheets>
     <sheet name="ASSESSMENTS" sheetId="1" r:id="rId1"/>
@@ -45,15 +45,9 @@
     <t>Longitude</t>
   </si>
   <si>
-    <t>INDUSTRY</t>
-  </si>
-  <si>
     <t>Location</t>
   </si>
   <si>
-    <t xml:space="preserve">Industry </t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
@@ -72,9 +66,6 @@
     <t>End</t>
   </si>
   <si>
-    <t>SUPPLIERS</t>
-  </si>
-  <si>
     <t>Add as many suppliers (Name, Latitude, Longitude) as needed to the right</t>
   </si>
   <si>
@@ -82,6 +73,15 @@
   </si>
   <si>
     <t>industry 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Site </t>
+  </si>
+  <si>
+    <t>SITE</t>
+  </si>
+  <si>
+    <t>SUB-SUPPLIERS</t>
   </si>
 </sst>
 </file>
@@ -562,8 +562,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{155DBE8A-0346-4315-8D01-639509365F15}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -579,7 +579,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -587,24 +587,24 @@
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C2" s="5"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B4" s="3">
         <v>37035</v>
@@ -626,8 +626,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8B8E9D9-9D28-4A7A-8C86-9EFD3A6132E9}">
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -638,13 +638,13 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
       <c r="D1" s="9"/>
       <c r="E1" s="7" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F1" s="8"/>
       <c r="G1" s="8"/>
@@ -656,11 +656,11 @@
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="10" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D2" s="11"/>
       <c r="E2" s="12" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F2" s="13"/>
       <c r="G2" s="13"/>
@@ -670,10 +670,10 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>0</v>
@@ -682,7 +682,7 @@
         <v>1</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>0</v>
@@ -691,7 +691,7 @@
         <v>1</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>0</v>
@@ -702,10 +702,10 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C4" s="4">
         <v>44.659449000000002</v>

</xml_diff>